<commit_message>
all sensors working now
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -381,7 +381,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -414,22 +414,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>22.83</v>
+        <v>28.89</v>
       </c>
       <c r="E2" t="n">
-        <v>21.7</v>
+        <v>24.12</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -437,22 +437,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="n">
-        <v>22.83</v>
+        <v>28.63</v>
       </c>
       <c r="E3" t="n">
-        <v>21.74</v>
+        <v>24.09</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -460,22 +460,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="n">
-        <v>22.77</v>
+        <v>28.6</v>
       </c>
       <c r="E4" t="n">
-        <v>21.67</v>
+        <v>23.96</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -483,22 +483,22 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="n">
-        <v>22.8</v>
+        <v>28.25</v>
       </c>
       <c r="E5" t="n">
-        <v>21.7</v>
+        <v>23.86</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -506,22 +506,22 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" t="n">
-        <v>22.77</v>
+        <v>27.99</v>
       </c>
       <c r="E6" t="n">
-        <v>21.83</v>
+        <v>23.86</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G6" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -529,22 +529,22 @@
         <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="n">
-        <v>22.83</v>
+        <v>27.67</v>
       </c>
       <c r="E7" t="n">
-        <v>21.7</v>
+        <v>23.57</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -552,22 +552,22 @@
         <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="n">
-        <v>22.8</v>
+        <v>27.25</v>
       </c>
       <c r="E8" t="n">
-        <v>21.67</v>
+        <v>23.44</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -575,22 +575,22 @@
         <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="n">
-        <v>22.83</v>
+        <v>26.86</v>
       </c>
       <c r="E9" t="n">
-        <v>21.67</v>
+        <v>23.19</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -598,22 +598,22 @@
         <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="n">
-        <v>22.77</v>
+        <v>26.7</v>
       </c>
       <c r="E10" t="n">
-        <v>21.61</v>
+        <v>23.09</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -621,22 +621,22 @@
         <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="n">
-        <v>22.8</v>
+        <v>26.57</v>
       </c>
       <c r="E11" t="n">
-        <v>21.74</v>
+        <v>23.06</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G11" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -644,22 +644,22 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="n">
-        <v>22.83</v>
+        <v>26.41</v>
       </c>
       <c r="E12" t="n">
-        <v>21.61</v>
+        <v>23.19</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G12" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -667,22 +667,22 @@
         <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" t="n">
-        <v>22.83</v>
+        <v>26.44</v>
       </c>
       <c r="E13" t="n">
-        <v>21.74</v>
+        <v>23.22</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G13" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -690,22 +690,22 @@
         <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" t="n">
-        <v>22.83</v>
+        <v>26.38</v>
       </c>
       <c r="E14" t="n">
-        <v>21.7</v>
+        <v>23.19</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G14" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -713,22 +713,1195 @@
         <v>1</v>
       </c>
       <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="n">
+        <v>22</v>
+      </c>
+      <c r="D15" t="n">
+        <v>26.25</v>
+      </c>
+      <c r="E15" t="n">
+        <v>23.19</v>
+      </c>
+      <c r="F15" t="n">
+        <v>17</v>
+      </c>
+      <c r="G15" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" t="n">
+        <v>22</v>
+      </c>
+      <c r="D16" t="n">
+        <v>26.28</v>
+      </c>
+      <c r="E16" t="n">
+        <v>23.19</v>
+      </c>
+      <c r="F16" t="n">
+        <v>17</v>
+      </c>
+      <c r="G16" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="n">
+        <v>14</v>
+      </c>
+      <c r="C17" t="n">
+        <v>22</v>
+      </c>
+      <c r="D17" t="n">
+        <v>26.28</v>
+      </c>
+      <c r="E17" t="n">
+        <v>23.38</v>
+      </c>
+      <c r="F17" t="n">
+        <v>17</v>
+      </c>
+      <c r="G17" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" t="n">
+        <v>14</v>
+      </c>
+      <c r="C18" t="n">
+        <v>22</v>
+      </c>
+      <c r="D18" t="n">
+        <v>26.05</v>
+      </c>
+      <c r="E18" t="n">
+        <v>23.22</v>
+      </c>
+      <c r="F18" t="n">
+        <v>17</v>
+      </c>
+      <c r="G18" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="n">
+        <v>14</v>
+      </c>
+      <c r="C19" t="n">
+        <v>22</v>
+      </c>
+      <c r="D19" t="n">
+        <v>26.12</v>
+      </c>
+      <c r="E19" t="n">
+        <v>23.28</v>
+      </c>
+      <c r="F19" t="n">
+        <v>17</v>
+      </c>
+      <c r="G19" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" t="n">
+        <v>14</v>
+      </c>
+      <c r="C20" t="n">
+        <v>22</v>
+      </c>
+      <c r="D20" t="n">
+        <v>25.99</v>
+      </c>
+      <c r="E20" t="n">
+        <v>23.57</v>
+      </c>
+      <c r="F20" t="n">
+        <v>17</v>
+      </c>
+      <c r="G20" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="n">
+        <v>14</v>
+      </c>
+      <c r="C21" t="n">
+        <v>22</v>
+      </c>
+      <c r="D21" t="n">
+        <v>25.76</v>
+      </c>
+      <c r="E21" t="n">
+        <v>23.35</v>
+      </c>
+      <c r="F21" t="n">
+        <v>17</v>
+      </c>
+      <c r="G21" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" t="n">
+        <v>14</v>
+      </c>
+      <c r="C22" t="n">
+        <v>22</v>
+      </c>
+      <c r="D22" t="n">
+        <v>25.7</v>
+      </c>
+      <c r="E22" t="n">
+        <v>23.57</v>
+      </c>
+      <c r="F22" t="n">
+        <v>17</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" t="n">
+        <v>14</v>
+      </c>
+      <c r="C23" t="n">
+        <v>22</v>
+      </c>
+      <c r="D23" t="n">
+        <v>25.7</v>
+      </c>
+      <c r="E23" t="n">
+        <v>23.48</v>
+      </c>
+      <c r="F23" t="n">
+        <v>18</v>
+      </c>
+      <c r="G23" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" t="n">
+        <v>14</v>
+      </c>
+      <c r="C24" t="n">
+        <v>22</v>
+      </c>
+      <c r="D24" t="n">
+        <v>26.15</v>
+      </c>
+      <c r="E24" t="n">
+        <v>23.44</v>
+      </c>
+      <c r="F24" t="n">
+        <v>17</v>
+      </c>
+      <c r="G24" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" t="n">
+        <v>14</v>
+      </c>
+      <c r="C25" t="n">
+        <v>22</v>
+      </c>
+      <c r="D25" t="n">
+        <v>26.57</v>
+      </c>
+      <c r="E25" t="n">
+        <v>23.51</v>
+      </c>
+      <c r="F25" t="n">
+        <v>17</v>
+      </c>
+      <c r="G25" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" t="n">
+        <v>14</v>
+      </c>
+      <c r="C26" t="n">
+        <v>22</v>
+      </c>
+      <c r="D26" t="n">
+        <v>26.73</v>
+      </c>
+      <c r="E26" t="n">
+        <v>23.61</v>
+      </c>
+      <c r="F26" t="n">
+        <v>17</v>
+      </c>
+      <c r="G26" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" t="n">
+        <v>14</v>
+      </c>
+      <c r="C27" t="n">
+        <v>22</v>
+      </c>
+      <c r="D27" t="n">
+        <v>26.96</v>
+      </c>
+      <c r="E27" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="F27" t="n">
+        <v>17</v>
+      </c>
+      <c r="G27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B28" t="n">
+        <v>14</v>
+      </c>
+      <c r="C28" t="n">
+        <v>22</v>
+      </c>
+      <c r="D28" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="E28" t="n">
+        <v>23.96</v>
+      </c>
+      <c r="F28" t="n">
+        <v>17</v>
+      </c>
+      <c r="G28" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" t="n">
+        <v>14</v>
+      </c>
+      <c r="C29" t="n">
+        <v>22</v>
+      </c>
+      <c r="D29" t="n">
+        <v>27.76</v>
+      </c>
+      <c r="E29" t="n">
+        <v>24.41</v>
+      </c>
+      <c r="F29" t="n">
+        <v>17</v>
+      </c>
+      <c r="G29" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" t="n">
+        <v>14</v>
+      </c>
+      <c r="C30" t="n">
+        <v>22</v>
+      </c>
+      <c r="D30" t="n">
+        <v>28.18</v>
+      </c>
+      <c r="E30" t="n">
+        <v>24.48</v>
+      </c>
+      <c r="F30" t="n">
+        <v>18</v>
+      </c>
+      <c r="G30" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" t="n">
+        <v>14</v>
+      </c>
+      <c r="C31" t="n">
+        <v>22</v>
+      </c>
+      <c r="D31" t="n">
+        <v>28.25</v>
+      </c>
+      <c r="E31" t="n">
+        <v>24.48</v>
+      </c>
+      <c r="F31" t="n">
+        <v>18</v>
+      </c>
+      <c r="G31" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B32" t="n">
+        <v>14</v>
+      </c>
+      <c r="C32" t="n">
+        <v>22</v>
+      </c>
+      <c r="D32" t="n">
+        <v>28.37</v>
+      </c>
+      <c r="E32" t="n">
+        <v>24.6</v>
+      </c>
+      <c r="F32" t="n">
+        <v>18</v>
+      </c>
+      <c r="G32" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B33" t="n">
+        <v>14</v>
+      </c>
+      <c r="C33" t="n">
+        <v>22</v>
+      </c>
+      <c r="D33" t="n">
+        <v>28.63</v>
+      </c>
+      <c r="E33" t="n">
+        <v>24.64</v>
+      </c>
+      <c r="F33" t="n">
+        <v>18</v>
+      </c>
+      <c r="G33" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" t="n">
+        <v>14</v>
+      </c>
+      <c r="C34" t="n">
+        <v>22</v>
+      </c>
+      <c r="D34" t="n">
+        <v>29.08</v>
+      </c>
+      <c r="E34" t="n">
+        <v>24.83</v>
+      </c>
+      <c r="F34" t="n">
+        <v>18</v>
+      </c>
+      <c r="G34" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B35" t="n">
+        <v>14</v>
+      </c>
+      <c r="C35" t="n">
+        <v>22</v>
+      </c>
+      <c r="D35" t="n">
+        <v>29.6</v>
+      </c>
+      <c r="E35" t="n">
+        <v>24.99</v>
+      </c>
+      <c r="F35" t="n">
+        <v>18</v>
+      </c>
+      <c r="G35" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B36" t="n">
+        <v>14</v>
+      </c>
+      <c r="C36" t="n">
+        <v>22</v>
+      </c>
+      <c r="D36" t="n">
+        <v>29.83</v>
+      </c>
+      <c r="E36" t="n">
+        <v>25.38</v>
+      </c>
+      <c r="F36" t="n">
+        <v>18</v>
+      </c>
+      <c r="G36" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B37" t="n">
+        <v>14</v>
+      </c>
+      <c r="C37" t="n">
+        <v>22</v>
+      </c>
+      <c r="D37" t="n">
+        <v>30.21</v>
+      </c>
+      <c r="E37" t="n">
+        <v>25.44</v>
+      </c>
+      <c r="F37" t="n">
+        <v>18</v>
+      </c>
+      <c r="G37" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B38" t="n">
+        <v>14</v>
+      </c>
+      <c r="C38" t="n">
+        <v>22</v>
+      </c>
+      <c r="D38" t="n">
+        <v>30.53</v>
+      </c>
+      <c r="E38" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="F38" t="n">
+        <v>17</v>
+      </c>
+      <c r="G38" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" t="n">
+        <v>14</v>
+      </c>
+      <c r="C39" t="n">
+        <v>22</v>
+      </c>
+      <c r="D39" t="n">
+        <v>30.76</v>
+      </c>
+      <c r="E39" t="n">
+        <v>25.6</v>
+      </c>
+      <c r="F39" t="n">
+        <v>17</v>
+      </c>
+      <c r="G39" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B40" t="n">
+        <v>14</v>
+      </c>
+      <c r="C40" t="n">
+        <v>22</v>
+      </c>
+      <c r="D40" t="n">
+        <v>30.82</v>
+      </c>
+      <c r="E40" t="n">
+        <v>25.7</v>
+      </c>
+      <c r="F40" t="n">
+        <v>17</v>
+      </c>
+      <c r="G40" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B41" t="n">
+        <v>14</v>
+      </c>
+      <c r="C41" t="n">
+        <v>22</v>
+      </c>
+      <c r="D41" t="n">
+        <v>31.28</v>
+      </c>
+      <c r="E41" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="F41" t="n">
+        <v>17</v>
+      </c>
+      <c r="G41" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B42" t="n">
+        <v>14</v>
+      </c>
+      <c r="C42" t="n">
+        <v>22</v>
+      </c>
+      <c r="D42" t="n">
+        <v>31.5</v>
+      </c>
+      <c r="E42" t="n">
+        <v>26.22</v>
+      </c>
+      <c r="F42" t="n">
+        <v>17</v>
+      </c>
+      <c r="G42" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B43" t="n">
+        <v>14</v>
+      </c>
+      <c r="C43" t="n">
+        <v>22</v>
+      </c>
+      <c r="D43" t="n">
+        <v>31.57</v>
+      </c>
+      <c r="E43" t="n">
+        <v>25.99</v>
+      </c>
+      <c r="F43" t="n">
+        <v>17</v>
+      </c>
+      <c r="G43" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B44" t="n">
+        <v>14</v>
+      </c>
+      <c r="C44" t="n">
+        <v>22</v>
+      </c>
+      <c r="D44" t="n">
+        <v>31.66</v>
+      </c>
+      <c r="E44" t="n">
+        <v>26.02</v>
+      </c>
+      <c r="F44" t="n">
+        <v>17</v>
+      </c>
+      <c r="G44" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B45" t="n">
+        <v>14</v>
+      </c>
+      <c r="C45" t="n">
+        <v>22</v>
+      </c>
+      <c r="D45" t="n">
+        <v>31.79</v>
+      </c>
+      <c r="E45" t="n">
+        <v>26.25</v>
+      </c>
+      <c r="F45" t="n">
+        <v>17</v>
+      </c>
+      <c r="G45" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B46" t="n">
+        <v>14</v>
+      </c>
+      <c r="C46" t="n">
+        <v>22</v>
+      </c>
+      <c r="D46" t="n">
+        <v>31.79</v>
+      </c>
+      <c r="E46" t="n">
+        <v>26.28</v>
+      </c>
+      <c r="F46" t="n">
+        <v>17</v>
+      </c>
+      <c r="G46" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B47" t="n">
+        <v>14</v>
+      </c>
+      <c r="C47" t="n">
+        <v>22</v>
+      </c>
+      <c r="D47" t="n">
+        <v>31.82</v>
+      </c>
+      <c r="E47" t="n">
+        <v>26.28</v>
+      </c>
+      <c r="F47" t="n">
+        <v>17</v>
+      </c>
+      <c r="G47" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B48" t="n">
+        <v>14</v>
+      </c>
+      <c r="C48" t="n">
+        <v>22</v>
+      </c>
+      <c r="D48" t="n">
+        <v>31.76</v>
+      </c>
+      <c r="E48" t="n">
+        <v>25.96</v>
+      </c>
+      <c r="F48" t="n">
+        <v>17</v>
+      </c>
+      <c r="G48" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B49" t="n">
+        <v>14</v>
+      </c>
+      <c r="C49" t="n">
+        <v>22</v>
+      </c>
+      <c r="D49" t="n">
+        <v>31.86</v>
+      </c>
+      <c r="E49" t="n">
+        <v>26.38</v>
+      </c>
+      <c r="F49" t="n">
+        <v>17</v>
+      </c>
+      <c r="G49" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B50" t="n">
         <v>13</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C50" t="n">
         <v>23</v>
       </c>
-      <c r="D15" t="n">
-        <v>22.8</v>
-      </c>
-      <c r="E15" t="n">
-        <v>21.7</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" t="n">
-        <v>2</v>
+      <c r="D50" t="n">
+        <v>32.24</v>
+      </c>
+      <c r="E50" t="n">
+        <v>26.34</v>
+      </c>
+      <c r="F50" t="n">
+        <v>18</v>
+      </c>
+      <c r="G50" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B51" t="n">
+        <v>13</v>
+      </c>
+      <c r="C51" t="n">
+        <v>23</v>
+      </c>
+      <c r="D51" t="n">
+        <v>32.21</v>
+      </c>
+      <c r="E51" t="n">
+        <v>26.34</v>
+      </c>
+      <c r="F51" t="n">
+        <v>17</v>
+      </c>
+      <c r="G51" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B52" t="n">
+        <v>13</v>
+      </c>
+      <c r="C52" t="n">
+        <v>23</v>
+      </c>
+      <c r="D52" t="n">
+        <v>32.24</v>
+      </c>
+      <c r="E52" t="n">
+        <v>26.38</v>
+      </c>
+      <c r="F52" t="n">
+        <v>17</v>
+      </c>
+      <c r="G52" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B53" t="n">
+        <v>13</v>
+      </c>
+      <c r="C53" t="n">
+        <v>23</v>
+      </c>
+      <c r="D53" t="n">
+        <v>32.44</v>
+      </c>
+      <c r="E53" t="n">
+        <v>26.73</v>
+      </c>
+      <c r="F53" t="n">
+        <v>17</v>
+      </c>
+      <c r="G53" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B54" t="n">
+        <v>13</v>
+      </c>
+      <c r="C54" t="n">
+        <v>23</v>
+      </c>
+      <c r="D54" t="n">
+        <v>32.56</v>
+      </c>
+      <c r="E54" t="n">
+        <v>26.63</v>
+      </c>
+      <c r="F54" t="n">
+        <v>17</v>
+      </c>
+      <c r="G54" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B55" t="n">
+        <v>13</v>
+      </c>
+      <c r="C55" t="n">
+        <v>23</v>
+      </c>
+      <c r="D55" t="n">
+        <v>32.79</v>
+      </c>
+      <c r="E55" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="F55" t="n">
+        <v>17</v>
+      </c>
+      <c r="G55" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B56" t="n">
+        <v>13</v>
+      </c>
+      <c r="C56" t="n">
+        <v>23</v>
+      </c>
+      <c r="D56" t="n">
+        <v>33.05</v>
+      </c>
+      <c r="E56" t="n">
+        <v>26.96</v>
+      </c>
+      <c r="F56" t="n">
+        <v>17</v>
+      </c>
+      <c r="G56" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B57" t="n">
+        <v>13</v>
+      </c>
+      <c r="C57" t="n">
+        <v>23</v>
+      </c>
+      <c r="D57" t="n">
+        <v>33.4</v>
+      </c>
+      <c r="E57" t="n">
+        <v>27.21</v>
+      </c>
+      <c r="F57" t="n">
+        <v>17</v>
+      </c>
+      <c r="G57" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B58" t="n">
+        <v>13</v>
+      </c>
+      <c r="C58" t="n">
+        <v>23</v>
+      </c>
+      <c r="D58" t="n">
+        <v>33.53</v>
+      </c>
+      <c r="E58" t="n">
+        <v>27.02</v>
+      </c>
+      <c r="F58" t="n">
+        <v>17</v>
+      </c>
+      <c r="G58" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B59" t="n">
+        <v>13</v>
+      </c>
+      <c r="C59" t="n">
+        <v>23</v>
+      </c>
+      <c r="D59" t="n">
+        <v>33.66</v>
+      </c>
+      <c r="E59" t="n">
+        <v>27.15</v>
+      </c>
+      <c r="F59" t="n">
+        <v>17</v>
+      </c>
+      <c r="G59" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B60" t="n">
+        <v>13</v>
+      </c>
+      <c r="C60" t="n">
+        <v>23</v>
+      </c>
+      <c r="D60" t="n">
+        <v>33.82</v>
+      </c>
+      <c r="E60" t="n">
+        <v>27.25</v>
+      </c>
+      <c r="F60" t="n">
+        <v>17</v>
+      </c>
+      <c r="G60" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B61" t="n">
+        <v>13</v>
+      </c>
+      <c r="C61" t="n">
+        <v>23</v>
+      </c>
+      <c r="D61" t="n">
+        <v>34.05</v>
+      </c>
+      <c r="E61" t="n">
+        <v>27.25</v>
+      </c>
+      <c r="F61" t="n">
+        <v>17</v>
+      </c>
+      <c r="G61" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B62" t="n">
+        <v>13</v>
+      </c>
+      <c r="C62" t="n">
+        <v>23</v>
+      </c>
+      <c r="D62" t="n">
+        <v>34.24</v>
+      </c>
+      <c r="E62" t="n">
+        <v>27.38</v>
+      </c>
+      <c r="F62" t="n">
+        <v>136</v>
+      </c>
+      <c r="G62" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B63" t="n">
+        <v>13</v>
+      </c>
+      <c r="C63" t="n">
+        <v>23</v>
+      </c>
+      <c r="D63" t="n">
+        <v>34.43</v>
+      </c>
+      <c r="E63" t="n">
+        <v>27.57</v>
+      </c>
+      <c r="F63" t="n">
+        <v>17</v>
+      </c>
+      <c r="G63" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B64" t="n">
+        <v>13</v>
+      </c>
+      <c r="C64" t="n">
+        <v>23</v>
+      </c>
+      <c r="D64" t="n">
+        <v>34.79</v>
+      </c>
+      <c r="E64" t="n">
+        <v>27.67</v>
+      </c>
+      <c r="F64" t="n">
+        <v>17</v>
+      </c>
+      <c r="G64" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B65" t="n">
+        <v>13</v>
+      </c>
+      <c r="C65" t="n">
+        <v>23</v>
+      </c>
+      <c r="D65" t="n">
+        <v>34.92</v>
+      </c>
+      <c r="E65" t="n">
+        <v>27.83</v>
+      </c>
+      <c r="F65" t="n">
+        <v>17</v>
+      </c>
+      <c r="G65" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B66" t="n">
+        <v>13</v>
+      </c>
+      <c r="C66" t="n">
+        <v>23</v>
+      </c>
+      <c r="D66" t="n">
+        <v>35.14</v>
+      </c>
+      <c r="E66" t="n">
+        <v>27.89</v>
+      </c>
+      <c r="F66" t="n">
+        <v>17</v>
+      </c>
+      <c r="G66" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>